<commit_message>
Updated pcb to use 6mil clearance
at same time tracks got narrowed down to 8mil,
Added extra caps to radios (100nF)
</commit_message>
<xml_diff>
--- a/MysensorsGW.xlsx
+++ b/MysensorsGW.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="207">
   <si>
     <t xml:space="preserve">Source:</t>
   </si>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">Date:</t>
   </si>
   <si>
-    <t xml:space="preserve">tir 31 maj 2016 07:59:46 CEST</t>
+    <t xml:space="preserve">tir 07 jun 2016 19:16:10 CEST</t>
   </si>
   <si>
     <t xml:space="preserve">Tool:</t>
   </si>
   <si>
-    <t xml:space="preserve">Eeschema 4.1.0-alpha+201605272346+6836~44~ubuntu16.04.1-product</t>
+    <t xml:space="preserve">Eeschema 4.1.0-alpha+201606061201+6885~45~ubuntu16.04.1-product</t>
   </si>
   <si>
     <t xml:space="preserve">Generator:</t>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">MM027S020R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Itead recommended</t>
   </si>
   <si>
     <t xml:space="preserve">D1, </t>
@@ -736,7 +739,7 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1038,224 +1041,227 @@
       <c r="H13" s="0" t="s">
         <v>61</v>
       </c>
+      <c r="I13" s="0" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>47</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>41</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>47</v>
@@ -1263,203 +1269,203 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>41</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I27" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>47</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -1468,13 +1474,13 @@
         <v>91</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>47</v>
@@ -1482,7 +1488,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>4</v>
@@ -1491,422 +1497,428 @@
         <v>270</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>31</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>41</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I37" s="0" t="s">
         <v>41</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>47</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>41</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="B45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>189</v>
-      </c>
       <c r="F45" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I49" s="0" t="s">
         <v>41</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added RFM reset signal, and DIO5 for future use
</commit_message>
<xml_diff>
--- a/MysensorsGW.xlsx
+++ b/MysensorsGW.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="207">
   <si>
     <t xml:space="preserve">Source:</t>
   </si>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">Date:</t>
   </si>
   <si>
-    <t xml:space="preserve">tir 07 jun 2016 19:16:10 CEST</t>
+    <t xml:space="preserve">søn 03 jul 2016 22:33:14 CEST</t>
   </si>
   <si>
     <t xml:space="preserve">Tool:</t>
   </si>
   <si>
-    <t xml:space="preserve">Eeschema 4.1.0-alpha+201606061201+6885~45~ubuntu16.04.1-product</t>
+    <t xml:space="preserve">Eeschema 4.1.0-alpha+201606220817+6945~45~ubuntu16.04.1-product</t>
   </si>
   <si>
     <t xml:space="preserve">Generator:</t>
@@ -118,6 +118,9 @@
     <t xml:space="preserve">Pin_Headers:Pin_Header_Straight_1x02</t>
   </si>
   <si>
+    <t xml:space="preserve">NM</t>
+  </si>
+  <si>
     <t xml:space="preserve">C11, C2, C3, C4, C6, C13, C15, C1, C5, C21, C17, C10, C7, </t>
   </si>
   <si>
@@ -206,9 +209,6 @@
   </si>
   <si>
     <t xml:space="preserve">MM027S020R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Itead recommended</t>
   </si>
   <si>
     <t xml:space="preserve">D1, </t>
@@ -739,7 +739,7 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A29:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -885,163 +885,166 @@
       <c r="E7" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="G7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>13</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="I13" s="0" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1062,7 +1065,7 @@
         <v>66</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>67</v>
@@ -1085,7 +1088,7 @@
         <v>66</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>67</v>
@@ -1108,7 +1111,7 @@
         <v>66</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>67</v>
@@ -1131,7 +1134,7 @@
         <v>66</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>67</v>
@@ -1154,7 +1157,7 @@
         <v>66</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>67</v>
@@ -1186,7 +1189,7 @@
         <v>82</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J19" s="0" t="s">
         <v>83</v>
@@ -1218,7 +1221,7 @@
         <v>90</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J20" s="0" t="s">
         <v>91</v>
@@ -1243,6 +1246,12 @@
       <c r="F21" s="0" t="s">
         <v>95</v>
       </c>
+      <c r="G21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -1263,8 +1272,11 @@
       <c r="F22" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="I22" s="0" t="s">
-        <v>47</v>
+      <c r="G22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,8 +1298,11 @@
       <c r="F23" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>47</v>
+      <c r="G23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>67</v>
@@ -1319,7 +1334,7 @@
         <v>111</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>112</v>
@@ -1344,6 +1359,12 @@
       <c r="F25" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="G25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -1364,8 +1385,11 @@
       <c r="F26" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="I26" s="0" t="s">
-        <v>47</v>
+      <c r="G26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>67</v>
@@ -1390,8 +1414,11 @@
       <c r="F27" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="I27" s="0" t="s">
-        <v>47</v>
+      <c r="G27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L27" s="0" t="s">
         <v>67</v>
@@ -1416,8 +1443,11 @@
       <c r="F28" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="I28" s="0" t="s">
-        <v>47</v>
+      <c r="G28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="L28" s="0" t="s">
         <v>67</v>
@@ -1482,9 +1512,6 @@
       <c r="F31" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="I31" s="0" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -1551,9 +1578,6 @@
       <c r="H34" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="I34" s="0" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -1574,6 +1598,9 @@
       <c r="F35" s="0" t="s">
         <v>137</v>
       </c>
+      <c r="G35" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -1601,7 +1628,7 @@
         <v>147</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J36" s="0" t="s">
         <v>148</v>
@@ -1633,7 +1660,7 @@
         <v>153</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J37" s="0" t="s">
         <v>154</v>
@@ -1665,7 +1692,7 @@
         <v>159</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J38" s="0" t="s">
         <v>160</v>
@@ -1690,6 +1717,9 @@
       <c r="F39" s="0" t="s">
         <v>164</v>
       </c>
+      <c r="G39" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
@@ -1710,6 +1740,9 @@
       <c r="F40" s="0" t="s">
         <v>168</v>
       </c>
+      <c r="G40" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -1730,6 +1763,9 @@
       <c r="F41" s="0" t="s">
         <v>172</v>
       </c>
+      <c r="G41" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -1757,7 +1793,7 @@
         <v>179</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J42" s="0" t="s">
         <v>180</v>
@@ -1785,9 +1821,6 @@
       <c r="H43" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="I43" s="0" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -1808,6 +1841,9 @@
       <c r="F44" s="0" t="s">
         <v>105</v>
       </c>
+      <c r="G44" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -1828,6 +1864,9 @@
       <c r="F45" s="0" t="s">
         <v>105</v>
       </c>
+      <c r="G45" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -1848,6 +1887,9 @@
       <c r="F46" s="0" t="s">
         <v>105</v>
       </c>
+      <c r="G46" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -1868,6 +1910,9 @@
       <c r="F47" s="0" t="s">
         <v>105</v>
       </c>
+      <c r="G47" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
@@ -1888,6 +1933,9 @@
       <c r="F48" s="0" t="s">
         <v>105</v>
       </c>
+      <c r="G48" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -1912,7 +1960,7 @@
         <v>204</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J49" s="0" t="s">
         <v>205</v>

</xml_diff>